<commit_message>
WorkAt 2016/08/19 17:35 ・音乐插入功能
</commit_message>
<xml_diff>
--- a/SqlServerDBTable/音乐相关/T_TRACK_TYPE_MST.xlsx
+++ b/SqlServerDBTable/音乐相关/T_TRACK_TYPE_MST.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="T_TRACK_TYPE_MST" sheetId="1" r:id="rId1"/>
+    <sheet name="T_ALBUM_TYPE_MST" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>TRACK_TYPE_ID</t>
   </si>
@@ -259,6 +258,88 @@
       </rPr>
       <t>节目</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>片尾曲</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>片</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>头</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>曲</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OST</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>原声音</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>乐</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>广播</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>剧(角色)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>短声音集</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALBUM_TYPE_ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALBUM_TYPE_NAME</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -926,26 +1007,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>